<commit_message>
Added updated project artifacts
</commit_message>
<xml_diff>
--- a/project-artifacts/Product_Backlog-A074-Customer Relationship Management.xlsx
+++ b/project-artifacts/Product_Backlog-A074-Customer Relationship Management.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23730"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\289610\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48297F53-6F1E-41F4-8F9A-E5B2954E69E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="7" r:id="rId1"/>
@@ -86,7 +92,7 @@
     <definedName name="Type" localSheetId="3">#REF!</definedName>
     <definedName name="Type">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -94,6 +100,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -106,6 +113,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="163">
   <si>
+    <t>Customer Relationship Management</t>
+  </si>
+  <si>
     <t>Product Backlog</t>
   </si>
   <si>
@@ -119,6 +129,9 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Academy - Project Solutions</t>
   </si>
   <si>
     <t>Role</t>
@@ -312,43 +325,28 @@
 The release burn down chart would be automatically plotted based on the data given on the Release burn down table with story points remaining and the done.</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve"> Product Backlog                              Customer Relationship Management
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Project ID: A074                                 C3: Protected          Controlled Copy</t>
+    </r>
+  </si>
+  <si>
     <t>User Story Id</t>
   </si>
   <si>
+    <t>Priorities</t>
+  </si>
+  <si>
     <t>Story Point</t>
-  </si>
-  <si>
-    <t>Release Burndown</t>
-  </si>
-  <si>
-    <t>Only edit shaded columns, others are calculated</t>
-  </si>
-  <si>
-    <t>Story points</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Remaining</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Priorities</t>
-  </si>
-  <si>
-    <t>Academy - Project Solutions</t>
-  </si>
-  <si>
-    <t>Customer Relationship Management</t>
   </si>
   <si>
     <t>US_1</t>
@@ -377,6 +375,26 @@
   </si>
   <si>
     <t>Save the user details in the Database and allow user login</t>
+  </si>
+  <si>
+    <t>1. When the User clicks on the sign-up link, it should re-direct to registration form.
+2. User needs to fill some of the fields as mentioned below in requirement: 
+First Name, 
+Last Name, 
+DoB, 
+Gender, 
+Contact Number, 
+Email ID, 
+Job title, 
+Company, Country, 
+Employees (drop down listing employee count in comapany eg: 1-20, 21-200 etc)
+User Id,
+Password, 
+Confirm password
+3. Clicking ‘Submit’ should validate the datatype constraints for each field
+4. User failing to provide information on the mandatory fields be provided with an alert message – ‘Please update the highlighted mandatory field(s).’ Also, highlight the missed out field in red
+5. Post-successful field level validation, save the information in the database. 
+6. Upon saving the information in the database, display the message, ‘Your details are saved succesfully</t>
   </si>
   <si>
     <t>US_3</t>
@@ -423,7 +441,7 @@
 </t>
   </si>
   <si>
-    <t>Medium</t>
+    <t>Low</t>
   </si>
   <si>
     <t>US_5</t>
@@ -461,6 +479,33 @@
     <t>New Lead</t>
   </si>
   <si>
+    <t>On click of New Lead in the submenu of Leads should open modal popup from with below fields:
+-Lead Information
+Lead Owner(Auto fetch logged in user in read only textbox)
+Lead Status: (Dropdown: New, Contacted, Working, Qualified, Unqualified)
+Name: Salutation(Dropdown: with Mr.,Ms., Mrs., Dr.,Prof.)
+First Name,
+Last Name
+Phone
+Company
+Email
+-Address Information
+Street
+City
+State/Province
+Zip/Postal Code
+Country
+Website
+-Additional Information
+No. of Employees
+Lead Source (Dropdown: Advertisement,Employee Referral,External Referral,In-Store,Social,Other)
+Annual Revenue
+Industry (Dropdown: Agriculture,Chemical,Biotechnology,Banking etc)
+-Description Information
+Description
+Save Button : Validate the fields and save details in the database</t>
+  </si>
+  <si>
     <t>US_8</t>
   </si>
   <si>
@@ -470,6 +515,9 @@
     <t>On click of Lead in the main menu should open a page which lists Leads information in a gridview provided Search and export option</t>
   </si>
   <si>
+    <t>Medium</t>
+  </si>
+  <si>
     <t>US_9</t>
   </si>
   <si>
@@ -479,9 +527,6 @@
     <t>Import option should be provided above the grid and on click of the button should open the upload csv file window with the Download template given. On Upload button  click should import data in the database and must refresh the grid</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>US_10</t>
   </si>
   <si>
@@ -489,6 +534,35 @@
   </si>
   <si>
     <t>New Account</t>
+  </si>
+  <si>
+    <t>On click of New Account in the submenu of Accounts should open modal popup from with below fields:
+-Account Information
+Account Owner(Name of logged in user)
+Account Name (Entry and auto Search field for existing account)
+Phone
+Fax
+Website
+-Additional Information
+Type (Dropdown: Customer,Invester, Partner, Reseller )
+Employees
+Industry (Dropdown: Agriculture,Chemical,Biotechnology,Banking etc)
+Annual Revenue
+Description
+Billing Address
+Billing Street
+Billing City
+Billing State/Province
+Billing Zip/Postal Code
+Billing Country
+Shipping Address
+Shipping Street
+Shipping City
+Shipping State/Province
+Shipping Zip/Postal Code
+Shipping Country
+Copy Billing Address to Shipping Address(check box on click copy address)
+Save Button : Validate the fields and save details in the database</t>
   </si>
   <si>
     <t>US_11</t>
@@ -751,107 +825,10 @@
     <t>US_28</t>
   </si>
   <si>
-    <t>US_29</t>
-  </si>
-  <si>
-    <t>User logout</t>
-  </si>
-  <si>
-    <t>Log out from the website/ Dashboard</t>
-  </si>
-  <si>
-    <t>Logout button should be visible to the user at the top right side of the screen which on click ends user session</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> Product Backlog                              Customer Relationship Management
- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Project ID: A074                                 C3: Protected          Controlled Copy</t>
-    </r>
-  </si>
-  <si>
-    <t>1. When the User clicks on the sign-up link, it should re-direct to registration form.
-2. User needs to fill some of the fields as mentioned below in requirement: 
-First Name, 
-Last Name, 
-DoB, 
-Gender, 
-Contact Number, 
-Email ID, 
-Job title, 
-Company, Country, 
-Employees (drop down listing employee count in comapany eg: 1-20, 21-200 etc)
-User Id,
-Password, 
-Confirm password
-3. Clicking ‘Submit’ should validate the datatype constraints for each field
-4. User failing to provide information on the mandatory fields be provided with an alert message – ‘Please update the highlighted mandatory field(s).’ Also, highlight the missed out field in red
-5. Post-successful field level validation, save the information in the database. 
-6. Upon saving the information in the database, display the message, ‘Your details are saved succesfully</t>
-  </si>
-  <si>
-    <t>On click of New Lead in the submenu of Leads should open modal popup from with below fields:
--Lead Information
-Lead Owner(Auto fetch logged in user in read only textbox)
-Lead Status: (Dropdown: New, Contacted, Working, Qualified, Unqualified)
-Name: Salutation(Dropdown: with Mr.,Ms., Mrs., Dr.,Prof.)
-First Name,
-Last Name
-Phone
-Company
-Email
--Address Information
-Street
-City
-State/Province
-Zip/Postal Code
-Country
-Website
--Additional Information
-No. of Employees
-Lead Source (Dropdown: Advertisement,Employee Referral,External Referral,In-Store,Social,Other)
-Annual Revenue
-Industry (Dropdown: Agriculture,Chemical,Biotechnology,Banking etc)
--Description Information
-Description
-Save Button : Validate the fields and save details in the database</t>
-  </si>
-  <si>
-    <t>On click of New Account in the submenu of Accounts should open modal popup from with below fields:
--Account Information
-Account Owner(Name of logged in user)
-Account Name (Entry and auto Search field for existing account)
-Phone
-Fax
-Website
--Additional Information
-Type (Dropdown: Customer,Invester, Partner, Reseller )
-Employees
-Industry (Dropdown: Agriculture,Chemical,Biotechnology,Banking etc)
-Annual Revenue
-Description
-Billing Address
-Billing Street
-Billing City
-Billing State/Province
-Billing Zip/Postal Code
-Billing Country
-Shipping Address
-Shipping Street
-Shipping City
-Shipping State/Province
-Shipping Zip/Postal Code
-Shipping Country
-Copy Billing Address to Shipping Address(check box on click copy address)
-Save Button : Validate the fields and save details in the database</t>
+    <t>Password reset / Forgot User ID</t>
+  </si>
+  <si>
+    <t>As a user I should be able to reset password, retrieve User ID</t>
   </si>
   <si>
     <t>1-During registration, System should pop up three secret questions for Password recovery.
@@ -862,20 +839,50 @@
 6-On clicking Submit, the details should be saved to the Database</t>
   </si>
   <si>
-    <t>Password reset / Forgot User ID</t>
-  </si>
-  <si>
-    <t>As a user I should be able to reset password, retrieve User ID</t>
+    <t>US_29</t>
+  </si>
+  <si>
+    <t>User logout</t>
+  </si>
+  <si>
+    <t>Log out from the website/ Dashboard</t>
+  </si>
+  <si>
+    <t>Logout button should be visible to the user at the top right side of the screen which on click ends user session</t>
+  </si>
+  <si>
+    <t>Release Burndown</t>
+  </si>
+  <si>
+    <t>Only edit shaded columns, others are calculated</t>
+  </si>
+  <si>
+    <t>Story points</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1580,9 +1587,6 @@
     <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1593,6 +1597,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1690,151 +1697,151 @@
     </xf>
   </cellXfs>
   <cellStyles count="145">
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="143"/>
-    <cellStyle name="Normal 2 2" xfId="144"/>
+    <cellStyle name="Normal 2" xfId="143" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Normal 2 2" xfId="144" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1857,9 +1864,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-IN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1965,7 +1972,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-32C2-465F-AAB4-7E4A2D206234}"/>
             </c:ext>
@@ -2026,7 +2033,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-32C2-465F-AAB4-7E4A2D206234}"/>
             </c:ext>
@@ -2056,13 +2063,12 @@
           </c:upBars>
           <c:downBars/>
         </c:upDownBars>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="139859840"/>
-        <c:axId val="139870208"/>
+        <c:axId val="2144712184"/>
+        <c:axId val="2144717688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="139859840"/>
+        <c:axId val="2144712184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2106,7 +2112,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139870208"/>
+        <c:crossAx val="2144717688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2114,7 +2120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139870208"/>
+        <c:axId val="2144717688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2146,7 +2152,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139859840"/>
+        <c:crossAx val="2144712184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2183,7 +2189,7 @@
         <xdr:cNvPr id="2" name="Text Box 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2261,7 +2267,7 @@
         <xdr:cNvPr id="3" name="Line 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2315,7 +2321,7 @@
         <xdr:cNvPr id="4" name="Line 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2369,7 +2375,7 @@
         <xdr:cNvPr id="6" name="Text Box 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2430,7 +2436,7 @@
         <xdr:cNvPr id="7" name="Text Box 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2508,7 +2514,7 @@
         <xdr:cNvPr id="8" name="Line 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2562,7 +2568,7 @@
         <xdr:cNvPr id="9" name="Line 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2616,7 +2622,7 @@
         <xdr:cNvPr id="11" name="Text Box 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2694,7 +2700,7 @@
         <xdr:cNvPr id="12" name="Line 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2748,7 +2754,7 @@
         <xdr:cNvPr id="13" name="Line 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2802,7 +2808,7 @@
         <xdr:cNvPr id="15" name="Text Box 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2880,7 +2886,7 @@
         <xdr:cNvPr id="16" name="Picture 20" descr="content">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2954,7 +2960,7 @@
         <xdr:cNvPr id="17" name="Line 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3008,7 +3014,7 @@
         <xdr:cNvPr id="18" name="Line 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3062,7 +3068,7 @@
         <xdr:cNvPr id="21" name="Picture 20" descr="cid:image001.png@01D5D50E.B865DEC0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3120,7 +3126,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="cid:image001.png@01D5D50E.B865DEC0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3178,7 +3184,7 @@
         <xdr:cNvPr id="4" name="Picture 3" descr="cid:image001.png@01D5D50E.B865DEC0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3236,7 +3242,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3684,14 +3690,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
@@ -3703,7 +3709,7 @@
     <col min="8" max="16384" width="9.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="18.75" thickBot="1">
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
       <c r="D1" s="4"/>
@@ -3711,7 +3717,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="18">
       <c r="B2" s="34"/>
       <c r="C2" s="33"/>
       <c r="D2" s="32"/>
@@ -3719,7 +3725,7 @@
       <c r="F2" s="32"/>
       <c r="G2" s="31"/>
     </row>
-    <row r="3" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="18">
       <c r="B3" s="30"/>
       <c r="C3" s="29"/>
       <c r="D3" s="4"/>
@@ -3727,7 +3733,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="18">
       <c r="B4" s="30"/>
       <c r="C4" s="29"/>
       <c r="D4" s="4"/>
@@ -3735,7 +3741,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="18">
       <c r="B5" s="30"/>
       <c r="C5" s="29"/>
       <c r="D5" s="4"/>
@@ -3743,7 +3749,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" ht="20.25" customHeight="1">
       <c r="B6" s="82"/>
       <c r="C6" s="83"/>
       <c r="D6" s="83"/>
@@ -3751,7 +3757,7 @@
       <c r="F6" s="83"/>
       <c r="G6" s="84"/>
     </row>
-    <row r="7" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" ht="21" customHeight="1">
       <c r="B7" s="82"/>
       <c r="C7" s="83"/>
       <c r="D7" s="83"/>
@@ -3759,9 +3765,9 @@
       <c r="F7" s="83"/>
       <c r="G7" s="84"/>
     </row>
-    <row r="8" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" ht="29.25" customHeight="1">
       <c r="B8" s="88" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="C8" s="89"/>
       <c r="D8" s="89"/>
@@ -3769,7 +3775,7 @@
       <c r="F8" s="89"/>
       <c r="G8" s="90"/>
     </row>
-    <row r="9" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" ht="29.25" customHeight="1">
       <c r="B9" s="88"/>
       <c r="C9" s="89"/>
       <c r="D9" s="89"/>
@@ -3777,9 +3783,9 @@
       <c r="F9" s="89"/>
       <c r="G9" s="90"/>
     </row>
-    <row r="10" spans="2:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" ht="55.5" customHeight="1">
       <c r="B10" s="82" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="83"/>
       <c r="D10" s="83"/>
@@ -3787,7 +3793,7 @@
       <c r="F10" s="83"/>
       <c r="G10" s="84"/>
     </row>
-    <row r="11" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" ht="18.75" customHeight="1">
       <c r="B11" s="85"/>
       <c r="C11" s="86"/>
       <c r="D11" s="86"/>
@@ -3795,7 +3801,7 @@
       <c r="F11" s="86"/>
       <c r="G11" s="87"/>
     </row>
-    <row r="12" spans="2:7" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" ht="20.25">
       <c r="B12" s="76"/>
       <c r="C12" s="77"/>
       <c r="D12" s="77"/>
@@ -3803,7 +3809,7 @@
       <c r="F12" s="77"/>
       <c r="G12" s="78"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7">
       <c r="B13" s="28"/>
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
@@ -3811,7 +3817,7 @@
       <c r="F13" s="27"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7">
       <c r="B14" s="14"/>
       <c r="C14" s="25"/>
       <c r="D14" s="4"/>
@@ -3819,7 +3825,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7">
       <c r="B15" s="14"/>
       <c r="C15" s="25"/>
       <c r="D15" s="4"/>
@@ -3827,7 +3833,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7">
       <c r="B16" s="14"/>
       <c r="C16" s="25"/>
       <c r="D16" s="4"/>
@@ -3835,7 +3841,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="B17" s="14"/>
       <c r="C17" s="25"/>
       <c r="D17" s="4"/>
@@ -3843,7 +3849,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="B18" s="14"/>
       <c r="C18" s="25"/>
       <c r="D18" s="4"/>
@@ -3851,7 +3857,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="B19" s="14"/>
       <c r="C19" s="25"/>
       <c r="D19" s="4"/>
@@ -3859,7 +3865,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="14.25">
       <c r="B20" s="79"/>
       <c r="C20" s="80"/>
       <c r="D20" s="80"/>
@@ -3868,7 +3874,7 @@
       <c r="G20" s="81"/>
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="B21" s="14"/>
       <c r="C21" s="25"/>
       <c r="D21" s="4"/>
@@ -3876,7 +3882,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="B22" s="14"/>
       <c r="C22" s="25"/>
       <c r="D22" s="4"/>
@@ -3884,7 +3890,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="B23" s="14"/>
       <c r="C23" s="25"/>
       <c r="D23" s="4"/>
@@ -3892,38 +3898,38 @@
       <c r="F23" s="4"/>
       <c r="G23" s="24"/>
     </row>
-    <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="25.5">
       <c r="B24" s="14"/>
       <c r="C24" s="23"/>
       <c r="D24" s="23" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="21" customHeight="1">
       <c r="B25" s="14"/>
       <c r="C25" s="22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="E25" s="49"/>
       <c r="F25" s="49"/>
       <c r="G25" s="21"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="21" customHeight="1">
       <c r="B26" s="14"/>
       <c r="C26" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D26" s="49"/>
       <c r="E26" s="49"/>
@@ -3931,10 +3937,10 @@
       <c r="G26" s="21"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="21" customHeight="1">
       <c r="B27" s="14"/>
       <c r="C27" s="22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D27" s="50"/>
       <c r="E27" s="50"/>
@@ -3942,10 +3948,10 @@
       <c r="G27" s="21"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="21" customHeight="1">
       <c r="B28" s="14"/>
       <c r="C28" s="22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D28" s="51"/>
       <c r="E28" s="51"/>
@@ -3953,7 +3959,7 @@
       <c r="G28" s="21"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" s="15" customFormat="1">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="20"/>
@@ -3962,7 +3968,7 @@
       <c r="F29" s="17"/>
       <c r="G29" s="16"/>
     </row>
-    <row r="30" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" s="15" customFormat="1">
       <c r="A30" s="17"/>
       <c r="B30" s="19"/>
       <c r="C30" s="18"/>
@@ -3971,25 +3977,25 @@
       <c r="F30" s="17"/>
       <c r="G30" s="16"/>
     </row>
-    <row r="31" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="13.5" thickBot="1">
       <c r="B31" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="12.75" customHeight="1"/>
+    <row r="33" spans="2:4">
       <c r="B33" s="8"/>
       <c r="C33" s="7"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4">
       <c r="B34" s="5"/>
     </row>
   </sheetData>
@@ -4012,14 +4018,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="40" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="37" customWidth="1"/>
@@ -4030,9 +4036,9 @@
     <col min="7" max="16384" width="9.85546875" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" s="35" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" s="35" customFormat="1" ht="57" customHeight="1" thickBot="1">
       <c r="B1" s="93" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="94"/>
       <c r="D1" s="94"/>
@@ -4043,180 +4049,180 @@
       <c r="N1" s="36"/>
       <c r="O1" s="36"/>
     </row>
-    <row r="2" spans="2:15" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:15" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:15" ht="13.5" thickTop="1"/>
+    <row r="3" spans="2:15" ht="3" customHeight="1"/>
+    <row r="4" spans="2:15" ht="29.1" customHeight="1">
       <c r="C4" s="91" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" s="92"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:15">
       <c r="C5" s="39" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" s="39"/>
     </row>
-    <row r="6" spans="2:15" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:15" ht="93.75" customHeight="1">
       <c r="C6" s="95" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6" s="96"/>
     </row>
-    <row r="7" spans="2:15" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:15" ht="25.5">
       <c r="C7" s="43" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" ht="51" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="51">
       <c r="C8" s="43" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" ht="76.5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="76.5">
       <c r="C9" s="43" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="38.25">
       <c r="C10" s="43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" ht="76.5" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="76.5">
       <c r="C11" s="43" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="38.25">
       <c r="C12" s="43" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D12" s="47" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="51" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="51">
       <c r="C13" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="C14" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="75" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="C15" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="C16" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="75" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="25.5">
+      <c r="C17" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="29.1" customHeight="1">
+      <c r="C19" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="92"/>
+    </row>
+    <row r="20" spans="1:4" ht="25.5">
+      <c r="C20" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C14" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="71" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C15" s="43" t="s">
+      <c r="D20" s="75" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="39" customHeight="1">
+      <c r="C21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="75" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="46.5" customHeight="1">
+      <c r="C22" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="71" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C16" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="71" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C17" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="91" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="92"/>
-    </row>
-    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C20" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="71" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="71" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="71" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D22" s="75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="38.25">
       <c r="C23" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="71" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="D23" s="75" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="25.5">
       <c r="A24" s="41"/>
       <c r="B24" s="42"/>
       <c r="C24" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="71" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="127.5" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="D24" s="75" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="127.5">
       <c r="C25" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="71" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="354.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:4" ht="360.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="153" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>47</v>
+      </c>
+      <c r="D25" s="75" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="354.75" customHeight="1"/>
+    <row r="32" spans="1:4" ht="360.75" customHeight="1"/>
+    <row r="34" ht="153" customHeight="1"/>
+    <row r="37" ht="33" customHeight="1"/>
+    <row r="38" ht="33" customHeight="1"/>
+    <row r="39" ht="25.5" customHeight="1"/>
+    <row r="40" ht="25.5" customHeight="1"/>
+    <row r="41" ht="18" customHeight="1"/>
+    <row r="42" ht="25.5" customHeight="1"/>
+    <row r="43" ht="25.5" customHeight="1"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="4">
@@ -4226,10 +4232,10 @@
     <mergeCell ref="C6:D6"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:G1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:G1" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Simple,Average,Complex"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Functional, External Interface, User Interface,System Interface, Non functional"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4243,15 +4249,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="54" customWidth="1"/>
     <col min="2" max="3" width="17.42578125" style="54" customWidth="1"/>
@@ -4266,9 +4272,9 @@
     <col min="12" max="16384" width="8.85546875" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="52" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="52" customFormat="1" ht="57" customHeight="1" thickBot="1">
       <c r="A1" s="97" t="s">
-        <v>156</v>
+        <v>49</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -4284,7 +4290,7 @@
       <c r="M1" s="53"/>
       <c r="N1" s="53"/>
     </row>
-    <row r="2" spans="1:14" s="66" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="66" customFormat="1" ht="15.75" customHeight="1" thickTop="1">
       <c r="A2" s="99"/>
       <c r="B2" s="99"/>
       <c r="C2" s="99"/>
@@ -4294,633 +4300,711 @@
       <c r="G2" s="99"/>
       <c r="H2" s="100"/>
       <c r="I2" s="98" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J2" s="98"/>
       <c r="K2" s="98"/>
       <c r="L2" s="98"/>
       <c r="M2" s="57"/>
     </row>
-    <row r="3" spans="1:14" s="57" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="57" customFormat="1" ht="38.25">
       <c r="A3" s="56" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F3" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="68" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="48">
+      <c r="A4" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="70" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="68" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="68" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="48" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="F4" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="54">
+        <v>1</v>
+      </c>
+      <c r="H4" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="348">
+      <c r="A5" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="C5" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="E5" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="F5" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="54">
+        <v>1</v>
+      </c>
+      <c r="H5" s="54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="264">
+      <c r="A6" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="73" t="s">
+      <c r="B6" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="72" t="s">
+      <c r="C6" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="71" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="348" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
+      <c r="E6" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="F6" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="54">
+        <v>1</v>
+      </c>
+      <c r="H6" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="132">
+      <c r="A7" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="72" t="s">
+      <c r="B7" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="72" t="s">
-        <v>157</v>
-      </c>
-      <c r="F5" s="72" t="s">
+      <c r="C7" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="71" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="264" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="E7" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="F7" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="72" t="s">
+    </row>
+    <row r="8" spans="1:14" ht="48">
+      <c r="A8" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="73" t="s">
+      <c r="B8" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="132" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="C8" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="E8" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="72" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="73" t="s">
+      <c r="F8" s="71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="36">
+      <c r="A9" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="72" t="s">
+      <c r="B9" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="72" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="408">
+      <c r="A10" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="54">
+        <v>1</v>
+      </c>
+      <c r="H10" s="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="36">
+      <c r="A11" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="54"/>
+    </row>
+    <row r="12" spans="1:14" ht="60">
+      <c r="A12" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="54"/>
+    </row>
+    <row r="13" spans="1:14" ht="409.6">
+      <c r="A13" s="71" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="54">
+        <v>1</v>
+      </c>
+      <c r="H13" s="54">
+        <v>5</v>
+      </c>
+      <c r="J13" s="54"/>
+    </row>
+    <row r="14" spans="1:14" ht="36">
+      <c r="A14" s="71" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="48" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="72" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="72" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="73" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="72" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="36" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="73" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="72" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="408" x14ac:dyDescent="0.25">
-      <c r="A10" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="72" t="s">
+      <c r="B14" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="72" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="F10" s="72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="36" x14ac:dyDescent="0.25">
-      <c r="A11" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="72" t="s">
+      <c r="J14" s="54"/>
+    </row>
+    <row r="15" spans="1:14" ht="60">
+      <c r="A15" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="60">
+      <c r="A16" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="409.6">
+      <c r="A17" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="72" t="s">
+      <c r="G17" s="54">
+        <v>2</v>
+      </c>
+      <c r="H17" s="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="36">
+      <c r="A18" s="71" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="54">
+        <v>2</v>
+      </c>
+      <c r="H18" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="312">
+      <c r="A19" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="54">
+        <v>1</v>
+      </c>
+      <c r="H19" s="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60">
+      <c r="A20" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="E11" s="72" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="72" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" s="54"/>
-    </row>
-    <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="72" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="72" t="s">
+      <c r="F20" s="71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="48">
+      <c r="A21" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="72" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="72" t="s">
-        <v>94</v>
-      </c>
-      <c r="J12" s="54"/>
-    </row>
-    <row r="13" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="72" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="72" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="72" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="73" t="s">
-        <v>159</v>
-      </c>
-      <c r="F13" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="54"/>
-    </row>
-    <row r="14" spans="1:14" ht="36" x14ac:dyDescent="0.25">
-      <c r="A14" s="72" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="72" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="E14" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="72" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14" s="54"/>
-    </row>
-    <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="72" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="72" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="72" t="s">
-        <v>102</v>
-      </c>
-      <c r="E15" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="72" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="72" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="72" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" s="72" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="72" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="72" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="F17" s="72" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A18" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="C18" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="72" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="72" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="312" x14ac:dyDescent="0.25">
-      <c r="A19" s="72" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" s="72" t="s">
-        <v>112</v>
-      </c>
-      <c r="C19" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="72" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="F19" s="72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="72" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="72" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="72" t="s">
+    </row>
+    <row r="22" spans="1:8" ht="336">
+      <c r="A22" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="E20" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="72" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A21" s="72" t="s">
+      <c r="B22" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="72" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="72" t="s">
+      <c r="C22" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="72" t="s">
+      <c r="E22" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="F21" s="72" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="336" x14ac:dyDescent="0.25">
-      <c r="A22" s="72" t="s">
+      <c r="F22" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="54">
+        <v>2</v>
+      </c>
+      <c r="H22" s="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="36">
+      <c r="A23" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="72" t="s">
+      <c r="B23" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="C22" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="72" t="s">
+      <c r="C23" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="E22" s="72" t="s">
+      <c r="E23" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="F22" s="72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A23" s="72" t="s">
+      <c r="F23" s="71" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60">
+      <c r="A24" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="B23" s="72" t="s">
+      <c r="B24" s="71" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="72" t="s">
+      <c r="E24" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="276">
+      <c r="A25" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="E23" s="72" t="s">
+      <c r="B25" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="F23" s="72" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="72" t="s">
+      <c r="C25" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="72" t="s">
-        <v>125</v>
-      </c>
-      <c r="C24" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="72" t="s">
+      <c r="E25" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="72" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="276" x14ac:dyDescent="0.25">
-      <c r="A25" s="72" t="s">
+      <c r="F25" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="54">
+        <v>2</v>
+      </c>
+      <c r="H25" s="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="36">
+      <c r="A26" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B26" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="72" t="s">
+      <c r="C26" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="E25" s="72" t="s">
+      <c r="E26" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="F25" s="72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A26" s="72" t="s">
+      <c r="F26" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="54">
+        <v>2</v>
+      </c>
+      <c r="H26" s="54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60">
+      <c r="A27" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="72" t="s">
+      <c r="B27" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="71" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="72" t="s">
+      <c r="E27" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="48">
+      <c r="A28" s="71" t="s">
         <v>136</v>
       </c>
-      <c r="E26" s="72" t="s">
+      <c r="B28" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="F26" s="72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="72" t="s">
+      <c r="C28" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="B27" s="72" t="s">
-        <v>135</v>
-      </c>
-      <c r="C27" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="72" t="s">
+      <c r="E28" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="E27" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="72" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A28" s="72" t="s">
+      <c r="F28" s="71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="204">
+      <c r="A29" s="71" t="s">
         <v>140</v>
       </c>
-      <c r="B28" s="72" t="s">
+      <c r="B29" s="71" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="72" t="s">
+      <c r="E29" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="E28" s="72" t="s">
+      <c r="F29" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="54">
+        <v>2</v>
+      </c>
+      <c r="H29" s="54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="96">
+      <c r="A30" s="71" t="s">
         <v>143</v>
       </c>
-      <c r="F28" s="72" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="204" x14ac:dyDescent="0.25">
-      <c r="A29" s="72" t="s">
+      <c r="B30" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="72" t="s">
-        <v>141</v>
-      </c>
-      <c r="C29" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="72" t="s">
+      <c r="C30" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="E29" s="72" t="s">
+      <c r="E30" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="F29" s="72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="96" x14ac:dyDescent="0.25">
-      <c r="A30" s="72" t="s">
+      <c r="F30" s="71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="168">
+      <c r="A31" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="B30" s="72" t="s">
+      <c r="B31" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="72" t="s">
+      <c r="C31" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="74" t="s">
         <v>149</v>
       </c>
-      <c r="E30" s="72" t="s">
+      <c r="E31" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="F30" s="72" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="168" x14ac:dyDescent="0.25">
-      <c r="A31" s="72" t="s">
+      <c r="F31" s="73" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="36">
+      <c r="A32" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="75" t="s">
-        <v>161</v>
-      </c>
-      <c r="C31" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="75" t="s">
-        <v>162</v>
-      </c>
-      <c r="E31" s="72" t="s">
-        <v>160</v>
-      </c>
-      <c r="F31" s="74" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A32" s="72" t="s">
+      <c r="B32" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="B32" s="72" t="s">
+      <c r="C32" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="C32" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="72" t="s">
+      <c r="E32" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="E32" s="72" t="s">
-        <v>155</v>
-      </c>
-      <c r="F32" s="72" t="s">
-        <v>65</v>
+      <c r="F32" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="54">
+        <v>2</v>
+      </c>
+      <c r="H32" s="54">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -4936,13 +5020,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Functional, External Interface, User Interface,System Interface, Non functional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H81 L4:L80">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H81 L4:L80" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"1,2,3,5,8,13,21"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I88">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I88" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4958,14 +5042,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="59"/>
     <col min="2" max="2" width="10.85546875" style="59" bestFit="1" customWidth="1"/>
@@ -4976,54 +5060,54 @@
     <col min="8" max="16384" width="8.85546875" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="25.5">
       <c r="A1" s="58" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="103" t="s">
-        <v>50</v>
+        <v>156</v>
       </c>
       <c r="B2" s="103"/>
       <c r="C2" s="103"/>
       <c r="D2" s="103"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="104" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="C4" s="106"/>
       <c r="D4" s="106"/>
       <c r="E4" s="107" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F4" s="101" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="G4" s="101" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="13.5" thickBot="1">
       <c r="A5" s="105"/>
       <c r="B5" s="69" t="s">
-        <v>54</v>
+        <v>160</v>
       </c>
       <c r="C5" s="69" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D5" s="69" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E5" s="108"/>
       <c r="F5" s="102"/>
       <c r="G5" s="102"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="62">
         <v>1</v>
       </c>
@@ -5049,7 +5133,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="62">
         <v>2</v>
       </c>
@@ -5076,7 +5160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="62">
         <v>3</v>
       </c>
@@ -5103,14 +5187,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:3">
       <c r="C28" s="59" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3">
       <c r="C29" s="59" t="s">
-        <v>56</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -5124,7 +5208,7 @@
     <mergeCell ref="F4:F5"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>$C$28:$C$30</formula1>
     </dataValidation>
   </dataValidations>
@@ -5135,66 +5219,66 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9">
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10">
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11">
         <v>1000</v>
       </c>
@@ -5211,21 +5295,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9C735C9F3CD54A948D0AD38DF112BF" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11ad66446dc32c3b807414097220c56d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eac52b12-2228-488c-9d59-8a93d308b64e" xmlns:ns3="951c5514-b77c-4532-82d5-a05f2f7d58e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9337801316215d934d3adce979b41d8d" ns2:_="" ns3:_="">
     <xsd:import namespace="eac52b12-2228-488c-9d59-8a93d308b64e"/>
@@ -5442,46 +5517,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8575168F-6331-41DA-B879-8152475B9854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0C9F9C-98B5-480F-B2D6-CAE7CFAF0133}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0C9F9C-98B5-480F-B2D6-CAE7CFAF0133}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="eac52b12-2228-488c-9d59-8a93d308b64e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B228AAF5-D924-461D-A5C2-455DA6563D1C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B228AAF5-D924-461D-A5C2-455DA6563D1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="eac52b12-2228-488c-9d59-8a93d308b64e"/>
-    <ds:schemaRef ds:uri="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8575168F-6331-41DA-B879-8152475B9854}"/>
 </file>
</xml_diff>